<commit_message>
daniel_zepp month of planing upload
Former-commit-id: 0bb84c8b701c27e711cbdefcaa6e43470db7a900
</commit_message>
<xml_diff>
--- a/doc/1. Plan/Project_Lubycon.xlsx
+++ b/doc/1. Plan/Project_Lubycon.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="45" windowWidth="9615" windowHeight="4860" activeTab="1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
   <si>
     <t>15년</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -180,14 +180,46 @@
   </si>
   <si>
     <t>Back</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Front</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Daniel Zepot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">비밀번호 보안성 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>contents view slide show import</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>toggle btn  (다른곳을 누르면 닫히는)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>editer html, css작업 (JS는 할수있는만큼)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jumbotrone img resize query search</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>board</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,7 +259,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -306,6 +338,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="24">
     <border>
@@ -628,7 +666,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -740,6 +778,42 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="14" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="15" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="20" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -755,18 +829,24 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -776,31 +856,16 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -815,6 +880,11 @@
       <color rgb="FF00FF00"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -893,6 +963,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -927,6 +998,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1102,14 +1174,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N8"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="1" customWidth="1"/>
     <col min="2" max="2" width="18.625" customWidth="1"/>
@@ -1118,8 +1190,8 @@
     <col min="13" max="13" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="9.75" customHeight="1" thickBot="1"/>
-    <row r="2" spans="2:14" ht="33" customHeight="1" thickBot="1">
+    <row r="1" spans="2:14" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:14" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="33" t="s">
         <v>20</v>
       </c>
@@ -1160,37 +1232,37 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1">
+    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1">
         <v>2015</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="38" t="s">
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="38"/>
-      <c r="M3" s="39" t="s">
+      <c r="L3" s="50"/>
+      <c r="M3" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="40"/>
-    </row>
-    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1">
+      <c r="N3" s="52"/>
+    </row>
+    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1">
         <v>2016</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="41"/>
+      <c r="D4" s="53"/>
       <c r="E4" s="36" t="s">
         <v>14</v>
       </c>
@@ -1204,7 +1276,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="3"/>
     </row>
-    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1">
+    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1219,7 +1291,7 @@
       <c r="M5" s="2"/>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1">
+    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -1234,7 +1306,7 @@
       <c r="M6" s="2"/>
       <c r="N6" s="3"/>
     </row>
-    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1">
+    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1249,7 +1321,7 @@
       <c r="M7" s="2"/>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="5"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -1278,76 +1350,77 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AM23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AM29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="12.875" customWidth="1"/>
     <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
     <col min="5" max="39" width="3.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="17.25" thickBot="1"/>
-    <row r="2" spans="1:39">
-      <c r="A2" s="42" t="s">
+    <row r="1" spans="1:39" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A2" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46" t="s">
+      <c r="D2" s="60"/>
+      <c r="E2" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="55" t="s">
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="46"/>
-      <c r="S2" s="46"/>
-      <c r="T2" s="46"/>
-      <c r="U2" s="46"/>
-      <c r="V2" s="46"/>
-      <c r="W2" s="46"/>
-      <c r="X2" s="46"/>
-      <c r="Y2" s="46"/>
-      <c r="Z2" s="46"/>
-      <c r="AA2" s="46"/>
-      <c r="AB2" s="46"/>
-      <c r="AC2" s="46"/>
-      <c r="AD2" s="46"/>
-      <c r="AE2" s="46"/>
-      <c r="AF2" s="46"/>
-      <c r="AG2" s="46"/>
-      <c r="AH2" s="46"/>
-      <c r="AI2" s="46"/>
-      <c r="AJ2" s="46"/>
-      <c r="AK2" s="46"/>
-      <c r="AL2" s="46"/>
-      <c r="AM2" s="48"/>
-    </row>
-    <row r="3" spans="1:39">
-      <c r="A3" s="43"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="60"/>
+      <c r="S2" s="60"/>
+      <c r="T2" s="60"/>
+      <c r="U2" s="60"/>
+      <c r="V2" s="60"/>
+      <c r="W2" s="60"/>
+      <c r="X2" s="60"/>
+      <c r="Y2" s="60"/>
+      <c r="Z2" s="60"/>
+      <c r="AA2" s="60"/>
+      <c r="AB2" s="60"/>
+      <c r="AC2" s="60"/>
+      <c r="AD2" s="60"/>
+      <c r="AE2" s="60"/>
+      <c r="AF2" s="60"/>
+      <c r="AG2" s="60"/>
+      <c r="AH2" s="60"/>
+      <c r="AI2" s="60"/>
+      <c r="AJ2" s="60"/>
+      <c r="AK2" s="60"/>
+      <c r="AL2" s="60"/>
+      <c r="AM2" s="62"/>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A3" s="59"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
       <c r="E3" s="16">
         <v>28</v>
       </c>
@@ -1360,7 +1433,7 @@
       <c r="H3" s="15">
         <v>31</v>
       </c>
-      <c r="I3" s="56">
+      <c r="I3" s="40">
         <v>1</v>
       </c>
       <c r="J3" s="13">
@@ -1454,7 +1527,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:39">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
       <c r="B4" s="8"/>
       <c r="C4" s="19"/>
@@ -1495,14 +1568,14 @@
       <c r="AL4" s="20"/>
       <c r="AM4" s="22"/>
     </row>
-    <row r="5" spans="1:39" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="44" t="s">
+    <row r="5" spans="1:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="49" t="s">
+      <c r="C5" s="57" t="s">
         <v>33</v>
       </c>
       <c r="D5" s="11" t="s">
@@ -1511,8 +1584,8 @@
       <c r="E5" s="27"/>
       <c r="F5" s="28"/>
       <c r="G5" s="28"/>
-      <c r="H5" s="57"/>
-      <c r="I5" s="51"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="37"/>
       <c r="J5" s="17"/>
       <c r="K5" s="17"/>
       <c r="L5" s="17"/>
@@ -1544,18 +1617,18 @@
       <c r="AL5" s="17"/>
       <c r="AM5" s="18"/>
     </row>
-    <row r="6" spans="1:39" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="45"/>
-      <c r="B6" s="50"/>
-      <c r="C6" s="49"/>
+    <row r="6" spans="1:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="55"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="57"/>
       <c r="D6" s="11" t="s">
         <v>26</v>
       </c>
       <c r="E6" s="27"/>
       <c r="F6" s="28"/>
       <c r="G6" s="28"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="51"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="37"/>
       <c r="J6" s="17"/>
       <c r="K6" s="17"/>
       <c r="L6" s="17"/>
@@ -1587,18 +1660,18 @@
       <c r="AL6" s="17"/>
       <c r="AM6" s="18"/>
     </row>
-    <row r="7" spans="1:39" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="45"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="49"/>
+    <row r="7" spans="1:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="55"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="57"/>
       <c r="D7" s="11" t="s">
         <v>32</v>
       </c>
       <c r="E7" s="27"/>
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="51"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="37"/>
       <c r="J7" s="17"/>
       <c r="K7" s="17"/>
       <c r="L7" s="17"/>
@@ -1630,18 +1703,18 @@
       <c r="AL7" s="17"/>
       <c r="AM7" s="18"/>
     </row>
-    <row r="8" spans="1:39" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="45"/>
-      <c r="B8" s="50"/>
-      <c r="C8" s="49"/>
+    <row r="8" spans="1:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="55"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="57"/>
       <c r="D8" s="11" t="s">
         <v>29</v>
       </c>
       <c r="E8" s="27"/>
       <c r="F8" s="28"/>
       <c r="G8" s="28"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="51"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="37"/>
       <c r="J8" s="28"/>
       <c r="K8" s="28"/>
       <c r="L8" s="28"/>
@@ -1673,18 +1746,18 @@
       <c r="AL8" s="17"/>
       <c r="AM8" s="18"/>
     </row>
-    <row r="9" spans="1:39" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="45"/>
-      <c r="B9" s="50"/>
-      <c r="C9" s="49"/>
+    <row r="9" spans="1:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="55"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="57"/>
       <c r="D9" s="11" t="s">
         <v>31</v>
       </c>
       <c r="E9" s="27"/>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="51"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="37"/>
       <c r="J9" s="28"/>
       <c r="K9" s="28"/>
       <c r="L9" s="28"/>
@@ -1716,18 +1789,18 @@
       <c r="AL9" s="17"/>
       <c r="AM9" s="18"/>
     </row>
-    <row r="10" spans="1:39" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="45"/>
-      <c r="B10" s="50"/>
-      <c r="C10" s="49"/>
+    <row r="10" spans="1:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="55"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="57"/>
       <c r="D10" s="11" t="s">
         <v>30</v>
       </c>
       <c r="E10" s="27"/>
       <c r="F10" s="28"/>
       <c r="G10" s="28"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="51"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="37"/>
       <c r="J10" s="28"/>
       <c r="K10" s="28"/>
       <c r="L10" s="28"/>
@@ -1759,18 +1832,18 @@
       <c r="AL10" s="17"/>
       <c r="AM10" s="18"/>
     </row>
-    <row r="11" spans="1:39" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="45"/>
-      <c r="B11" s="50"/>
-      <c r="C11" s="49"/>
+    <row r="11" spans="1:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="55"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="57"/>
       <c r="D11" s="11" t="s">
         <v>28</v>
       </c>
       <c r="E11" s="27"/>
       <c r="F11" s="28"/>
       <c r="G11" s="28"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="51"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="37"/>
       <c r="J11" s="28"/>
       <c r="K11" s="28"/>
       <c r="L11" s="28"/>
@@ -1802,18 +1875,18 @@
       <c r="AL11" s="17"/>
       <c r="AM11" s="18"/>
     </row>
-    <row r="12" spans="1:39" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="45"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="49"/>
+    <row r="12" spans="1:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="55"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="57"/>
       <c r="D12" s="11" t="s">
         <v>27</v>
       </c>
       <c r="E12" s="27"/>
       <c r="F12" s="28"/>
       <c r="G12" s="28"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="51"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="37"/>
       <c r="J12" s="28"/>
       <c r="K12" s="28"/>
       <c r="L12" s="28"/>
@@ -1845,10 +1918,10 @@
       <c r="AL12" s="17"/>
       <c r="AM12" s="18"/>
     </row>
-    <row r="13" spans="1:39" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="45"/>
-      <c r="B13" s="50"/>
-      <c r="C13" s="49"/>
+    <row r="13" spans="1:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="55"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="57"/>
       <c r="D13" s="29" t="s">
         <v>38</v>
       </c>
@@ -1856,7 +1929,7 @@
       <c r="F13" s="31"/>
       <c r="G13" s="31"/>
       <c r="H13" s="32"/>
-      <c r="I13" s="52"/>
+      <c r="I13" s="38"/>
       <c r="J13" s="31"/>
       <c r="K13" s="31"/>
       <c r="L13" s="31"/>
@@ -1888,9 +1961,9 @@
       <c r="AL13" s="31"/>
       <c r="AM13" s="32"/>
     </row>
-    <row r="14" spans="1:39">
-      <c r="A14" s="45"/>
-      <c r="B14" s="50"/>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A14" s="55"/>
+      <c r="B14" s="56"/>
       <c r="C14" s="23"/>
       <c r="D14" s="24"/>
       <c r="E14" s="25"/>
@@ -1929,10 +2002,10 @@
       <c r="AL14" s="25"/>
       <c r="AM14" s="26"/>
     </row>
-    <row r="15" spans="1:39">
-      <c r="A15" s="45"/>
-      <c r="B15" s="50"/>
-      <c r="C15" s="49" t="s">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A15" s="55"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="57" t="s">
         <v>34</v>
       </c>
       <c r="D15" s="11" t="s">
@@ -1941,8 +2014,8 @@
       <c r="E15" s="27"/>
       <c r="F15" s="28"/>
       <c r="G15" s="28"/>
-      <c r="H15" s="57"/>
-      <c r="I15" s="51"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="37"/>
       <c r="J15" s="28"/>
       <c r="K15" s="28"/>
       <c r="L15" s="28"/>
@@ -1974,18 +2047,18 @@
       <c r="AL15" s="17"/>
       <c r="AM15" s="18"/>
     </row>
-    <row r="16" spans="1:39">
-      <c r="A16" s="45"/>
-      <c r="B16" s="50"/>
-      <c r="C16" s="49"/>
+    <row r="16" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A16" s="55"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="57"/>
       <c r="D16" s="11" t="s">
         <v>36</v>
       </c>
       <c r="E16" s="27"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
-      <c r="H16" s="57"/>
-      <c r="I16" s="51"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="37"/>
       <c r="J16" s="28"/>
       <c r="K16" s="28"/>
       <c r="L16" s="28"/>
@@ -2017,45 +2090,467 @@
       <c r="AL16" s="17"/>
       <c r="AM16" s="18"/>
     </row>
-    <row r="17" spans="8:39">
-      <c r="H17" s="53"/>
+    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="H17" s="39"/>
       <c r="AM17" s="10"/>
     </row>
-    <row r="18" spans="8:39">
-      <c r="H18" s="54"/>
-      <c r="AM18" s="10"/>
-    </row>
-    <row r="19" spans="8:39">
-      <c r="H19" s="54"/>
-      <c r="AM19" s="10"/>
-    </row>
-    <row r="20" spans="8:39">
-      <c r="H20" s="54"/>
-      <c r="AM20" s="10"/>
-    </row>
-    <row r="21" spans="8:39">
-      <c r="H21" s="54"/>
-      <c r="AM21" s="10"/>
-    </row>
-    <row r="22" spans="8:39">
-      <c r="H22" s="54"/>
-      <c r="AM22" s="10"/>
-    </row>
-    <row r="23" spans="8:39">
-      <c r="H23" s="54"/>
-      <c r="AM23" s="10"/>
+    <row r="18" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A18" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="56" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="57"/>
+      <c r="D18" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="27"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="17"/>
+      <c r="T18" s="17"/>
+      <c r="U18" s="17"/>
+      <c r="V18" s="17"/>
+      <c r="W18" s="17"/>
+      <c r="X18" s="17"/>
+      <c r="Y18" s="17"/>
+      <c r="Z18" s="17"/>
+      <c r="AA18" s="17"/>
+      <c r="AB18" s="17"/>
+      <c r="AC18" s="17"/>
+      <c r="AD18" s="17"/>
+      <c r="AE18" s="17"/>
+      <c r="AF18" s="17"/>
+      <c r="AG18" s="17"/>
+      <c r="AH18" s="17"/>
+      <c r="AI18" s="17"/>
+      <c r="AJ18" s="17"/>
+      <c r="AK18" s="17"/>
+      <c r="AL18" s="17"/>
+      <c r="AM18" s="18"/>
+    </row>
+    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A19" s="55"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="27"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="17"/>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="17"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="17"/>
+      <c r="U19" s="17"/>
+      <c r="V19" s="17"/>
+      <c r="W19" s="17"/>
+      <c r="X19" s="17"/>
+      <c r="Y19" s="17"/>
+      <c r="Z19" s="17"/>
+      <c r="AA19" s="17"/>
+      <c r="AB19" s="17"/>
+      <c r="AC19" s="17"/>
+      <c r="AD19" s="17"/>
+      <c r="AE19" s="17"/>
+      <c r="AF19" s="17"/>
+      <c r="AG19" s="17"/>
+      <c r="AH19" s="17"/>
+      <c r="AI19" s="17"/>
+      <c r="AJ19" s="17"/>
+      <c r="AK19" s="17"/>
+      <c r="AL19" s="17"/>
+      <c r="AM19" s="18"/>
+    </row>
+    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A20" s="55"/>
+      <c r="B20" s="56"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="27"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="17"/>
+      <c r="O20" s="17"/>
+      <c r="P20" s="17"/>
+      <c r="Q20" s="17"/>
+      <c r="R20" s="17"/>
+      <c r="S20" s="17"/>
+      <c r="T20" s="17"/>
+      <c r="U20" s="17"/>
+      <c r="V20" s="17"/>
+      <c r="W20" s="17"/>
+      <c r="X20" s="17"/>
+      <c r="Y20" s="17"/>
+      <c r="Z20" s="17"/>
+      <c r="AA20" s="17"/>
+      <c r="AB20" s="17"/>
+      <c r="AC20" s="17"/>
+      <c r="AD20" s="17"/>
+      <c r="AE20" s="17"/>
+      <c r="AF20" s="17"/>
+      <c r="AG20" s="17"/>
+      <c r="AH20" s="17"/>
+      <c r="AI20" s="17"/>
+      <c r="AJ20" s="17"/>
+      <c r="AK20" s="17"/>
+      <c r="AL20" s="17"/>
+      <c r="AM20" s="18"/>
+    </row>
+    <row r="21" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A21" s="55"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="64" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="65"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="65"/>
+      <c r="I21" s="65"/>
+      <c r="J21" s="65"/>
+      <c r="K21" s="65"/>
+      <c r="L21" s="65"/>
+      <c r="M21" s="65"/>
+      <c r="N21" s="65"/>
+      <c r="O21" s="65"/>
+      <c r="P21" s="65"/>
+      <c r="Q21" s="43"/>
+      <c r="R21" s="43"/>
+      <c r="S21" s="43"/>
+      <c r="T21" s="43"/>
+      <c r="U21" s="43"/>
+      <c r="V21" s="43"/>
+      <c r="W21" s="43"/>
+      <c r="X21" s="43"/>
+      <c r="Y21" s="43"/>
+      <c r="Z21" s="43"/>
+      <c r="AA21" s="43"/>
+      <c r="AB21" s="43"/>
+      <c r="AC21" s="43"/>
+      <c r="AD21" s="43"/>
+      <c r="AE21" s="43"/>
+      <c r="AF21" s="43"/>
+      <c r="AG21" s="43"/>
+      <c r="AH21" s="43"/>
+      <c r="AI21" s="43"/>
+      <c r="AJ21" s="43"/>
+      <c r="AK21" s="43"/>
+      <c r="AL21" s="43"/>
+      <c r="AM21" s="44"/>
+    </row>
+    <row r="22" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A22" s="55"/>
+      <c r="B22" s="56"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="27"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="28"/>
+      <c r="N22" s="28"/>
+      <c r="O22" s="28"/>
+      <c r="P22" s="28"/>
+      <c r="Q22" s="43"/>
+      <c r="R22" s="43"/>
+      <c r="S22" s="43"/>
+      <c r="T22" s="43"/>
+      <c r="U22" s="43"/>
+      <c r="V22" s="43"/>
+      <c r="W22" s="43"/>
+      <c r="X22" s="43"/>
+      <c r="Y22" s="43"/>
+      <c r="Z22" s="43"/>
+      <c r="AA22" s="43"/>
+      <c r="AB22" s="43"/>
+      <c r="AC22" s="43"/>
+      <c r="AD22" s="43"/>
+      <c r="AE22" s="43"/>
+      <c r="AF22" s="43"/>
+      <c r="AG22" s="43"/>
+      <c r="AH22" s="43"/>
+      <c r="AI22" s="43"/>
+      <c r="AJ22" s="43"/>
+      <c r="AK22" s="43"/>
+      <c r="AL22" s="43"/>
+      <c r="AM22" s="44"/>
+    </row>
+    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A23" s="55"/>
+      <c r="B23" s="56"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="45"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="46"/>
+      <c r="L23" s="46"/>
+      <c r="M23" s="46"/>
+      <c r="N23" s="46"/>
+      <c r="O23" s="46"/>
+      <c r="P23" s="46"/>
+      <c r="Q23" s="43"/>
+      <c r="R23" s="43"/>
+      <c r="S23" s="43"/>
+      <c r="T23" s="43"/>
+      <c r="U23" s="43"/>
+      <c r="V23" s="43"/>
+      <c r="W23" s="43"/>
+      <c r="X23" s="43"/>
+      <c r="Y23" s="43"/>
+      <c r="Z23" s="43"/>
+      <c r="AA23" s="43"/>
+      <c r="AB23" s="43"/>
+      <c r="AC23" s="43"/>
+      <c r="AD23" s="43"/>
+      <c r="AE23" s="43"/>
+      <c r="AF23" s="43"/>
+      <c r="AG23" s="43"/>
+      <c r="AH23" s="43"/>
+      <c r="AI23" s="43"/>
+      <c r="AJ23" s="43"/>
+      <c r="AK23" s="43"/>
+      <c r="AL23" s="43"/>
+      <c r="AM23" s="44"/>
+    </row>
+    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A24" s="55"/>
+      <c r="B24" s="56"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="27"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="28"/>
+      <c r="P24" s="28"/>
+      <c r="Q24" s="28"/>
+      <c r="R24" s="28"/>
+      <c r="S24" s="28"/>
+      <c r="T24" s="28"/>
+      <c r="U24" s="28"/>
+      <c r="V24" s="28"/>
+      <c r="W24" s="28"/>
+      <c r="X24" s="43"/>
+      <c r="Y24" s="43"/>
+      <c r="Z24" s="43"/>
+      <c r="AA24" s="43"/>
+      <c r="AB24" s="43"/>
+      <c r="AC24" s="43"/>
+      <c r="AD24" s="43"/>
+      <c r="AE24" s="43"/>
+      <c r="AF24" s="43"/>
+      <c r="AG24" s="43"/>
+      <c r="AH24" s="43"/>
+      <c r="AI24" s="43"/>
+      <c r="AJ24" s="43"/>
+      <c r="AK24" s="43"/>
+      <c r="AL24" s="43"/>
+      <c r="AM24" s="44"/>
+    </row>
+    <row r="25" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A25" s="55"/>
+      <c r="B25" s="56"/>
+      <c r="C25" s="57"/>
+    </row>
+    <row r="26" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A26" s="55"/>
+      <c r="B26" s="56"/>
+      <c r="C26" s="57"/>
+    </row>
+    <row r="27" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A27" s="55"/>
+      <c r="B27" s="56"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="25"/>
+      <c r="K27" s="25"/>
+      <c r="L27" s="25"/>
+      <c r="M27" s="25"/>
+      <c r="N27" s="25"/>
+      <c r="O27" s="25"/>
+      <c r="P27" s="25"/>
+      <c r="Q27" s="25"/>
+      <c r="R27" s="25"/>
+      <c r="S27" s="25"/>
+      <c r="T27" s="25"/>
+      <c r="U27" s="25"/>
+      <c r="V27" s="25"/>
+      <c r="W27" s="25"/>
+      <c r="X27" s="25"/>
+      <c r="Y27" s="25"/>
+      <c r="Z27" s="25"/>
+      <c r="AA27" s="25"/>
+      <c r="AB27" s="25"/>
+      <c r="AC27" s="25"/>
+      <c r="AD27" s="25"/>
+      <c r="AE27" s="25"/>
+      <c r="AF27" s="25"/>
+      <c r="AG27" s="25"/>
+      <c r="AH27" s="25"/>
+      <c r="AI27" s="25"/>
+      <c r="AJ27" s="25"/>
+      <c r="AK27" s="25"/>
+      <c r="AL27" s="25"/>
+      <c r="AM27" s="26"/>
+    </row>
+    <row r="28" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A28" s="55"/>
+      <c r="B28" s="56"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="E28" s="30"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="31"/>
+      <c r="K28" s="31"/>
+      <c r="L28" s="31"/>
+      <c r="M28" s="31"/>
+      <c r="N28" s="31"/>
+      <c r="O28" s="31"/>
+      <c r="P28" s="31"/>
+      <c r="Q28" s="31"/>
+      <c r="R28" s="31"/>
+      <c r="S28" s="31"/>
+      <c r="T28" s="31"/>
+      <c r="U28" s="31"/>
+      <c r="V28" s="31"/>
+      <c r="W28" s="31"/>
+      <c r="X28" s="31"/>
+      <c r="Y28" s="31"/>
+      <c r="Z28" s="31"/>
+      <c r="AA28" s="31"/>
+      <c r="AB28" s="31"/>
+      <c r="AC28" s="31"/>
+      <c r="AD28" s="31"/>
+      <c r="AE28" s="31"/>
+      <c r="AF28" s="31"/>
+      <c r="AG28" s="31"/>
+      <c r="AH28" s="31"/>
+      <c r="AI28" s="31"/>
+      <c r="AJ28" s="31"/>
+      <c r="AK28" s="31"/>
+      <c r="AL28" s="31"/>
+      <c r="AM28" s="32"/>
+    </row>
+    <row r="29" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A29" s="55"/>
+      <c r="B29" s="56"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29" s="30"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="31"/>
+      <c r="M29" s="31"/>
+      <c r="N29" s="31"/>
+      <c r="O29" s="31"/>
+      <c r="P29" s="31"/>
+      <c r="Q29" s="31"/>
+      <c r="R29" s="31"/>
+      <c r="S29" s="31"/>
+      <c r="T29" s="31"/>
+      <c r="U29" s="31"/>
+      <c r="V29" s="31"/>
+      <c r="W29" s="31"/>
+      <c r="X29" s="31"/>
+      <c r="Y29" s="31"/>
+      <c r="Z29" s="31"/>
+      <c r="AA29" s="31"/>
+      <c r="AB29" s="31"/>
+      <c r="AC29" s="31"/>
+      <c r="AD29" s="31"/>
+      <c r="AE29" s="31"/>
+      <c r="AF29" s="31"/>
+      <c r="AG29" s="31"/>
+      <c r="AH29" s="31"/>
+      <c r="AI29" s="31"/>
+      <c r="AJ29" s="31"/>
+      <c r="AK29" s="31"/>
+      <c r="AL29" s="31"/>
+      <c r="AM29" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A5:A16"/>
-    <mergeCell ref="B2:B3"/>
+  <mergeCells count="13">
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="I2:AM2"/>
     <mergeCell ref="C2:D3"/>
     <mergeCell ref="C5:C13"/>
     <mergeCell ref="B5:B16"/>
     <mergeCell ref="C15:C16"/>
+    <mergeCell ref="A18:A29"/>
+    <mergeCell ref="B18:B29"/>
+    <mergeCell ref="C18:C26"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A5:A16"/>
+    <mergeCell ref="B2:B3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2064,16 +2559,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>0</v>
       </c>
@@ -2081,7 +2576,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2119,7 +2614,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
create account password Argorizm end
Former-commit-id: 9090865d1cd15cc6d33e68e7292c2d99591a89c1
</commit_message>
<xml_diff>
--- a/doc/1. Plan/Project_Lubycon.xlsx
+++ b/doc/1. Plan/Project_Lubycon.xlsx
@@ -15,8 +15,86 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>daniel_zepot</author>
+  </authors>
+  <commentList>
+    <comment ref="AO2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>daniel_zepot:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+8자 이상 16자 이하              O
+1개이상의 문자포함              O
+3개이상의 반복된문자 금지     O
+알파벳만 가능                     O
+숫자만 가능                        O
+대,소문자 구분 없음              O
+공백 불가능(null문자열불가)    O</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AO12" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="major"/>
+          </rPr>
+          <t>daniel_zepot:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="major"/>
+          </rPr>
+          <t xml:space="preserve">
+알파벳만 가능(a-z) 
+숫자만 가능
+대,소문자 구분없음
+금지 닉네임 검사          O
+공백포함 불가
+특수문자 불가
+중복검사 (php)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
   <si>
     <t>15년</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -191,10 +269,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">비밀번호 보안성 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>contents view slide show import</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -212,6 +286,22 @@
   </si>
   <si>
     <t>board</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비밀번호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>닉네임</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비밀번호 보안성 (switch문)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>닉네임 관련 로직 (switch문)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -219,7 +309,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -257,6 +347,40 @@
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="81"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="81"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="81"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="81"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="15">
@@ -814,6 +938,15 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="20" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -829,44 +962,35 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1236,33 +1360,33 @@
       <c r="B3" s="1">
         <v>2015</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="50" t="s">
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="50"/>
-      <c r="M3" s="51" t="s">
+      <c r="L3" s="53"/>
+      <c r="M3" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="52"/>
+      <c r="N3" s="55"/>
     </row>
     <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1">
         <v>2016</v>
       </c>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="53"/>
+      <c r="D4" s="56"/>
       <c r="E4" s="36" t="s">
         <v>14</v>
       </c>
@@ -1350,11 +1474,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AO29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AT12" sqref="AT12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1364,63 +1488,66 @@
     <col min="5" max="39" width="3.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A2" s="58" t="s">
+    <row r="1" spans="1:41" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A2" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60" t="s">
+      <c r="D2" s="57"/>
+      <c r="E2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="63" t="s">
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
-      <c r="O2" s="60"/>
-      <c r="P2" s="60"/>
-      <c r="Q2" s="60"/>
-      <c r="R2" s="60"/>
-      <c r="S2" s="60"/>
-      <c r="T2" s="60"/>
-      <c r="U2" s="60"/>
-      <c r="V2" s="60"/>
-      <c r="W2" s="60"/>
-      <c r="X2" s="60"/>
-      <c r="Y2" s="60"/>
-      <c r="Z2" s="60"/>
-      <c r="AA2" s="60"/>
-      <c r="AB2" s="60"/>
-      <c r="AC2" s="60"/>
-      <c r="AD2" s="60"/>
-      <c r="AE2" s="60"/>
-      <c r="AF2" s="60"/>
-      <c r="AG2" s="60"/>
-      <c r="AH2" s="60"/>
-      <c r="AI2" s="60"/>
-      <c r="AJ2" s="60"/>
-      <c r="AK2" s="60"/>
-      <c r="AL2" s="60"/>
-      <c r="AM2" s="62"/>
-    </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A3" s="59"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
+      <c r="V2" s="57"/>
+      <c r="W2" s="57"/>
+      <c r="X2" s="57"/>
+      <c r="Y2" s="57"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="57"/>
+      <c r="AC2" s="57"/>
+      <c r="AD2" s="57"/>
+      <c r="AE2" s="57"/>
+      <c r="AF2" s="57"/>
+      <c r="AG2" s="57"/>
+      <c r="AH2" s="57"/>
+      <c r="AI2" s="57"/>
+      <c r="AJ2" s="57"/>
+      <c r="AK2" s="57"/>
+      <c r="AL2" s="57"/>
+      <c r="AM2" s="58"/>
+      <c r="AO2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A3" s="66"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
       <c r="E3" s="16">
         <v>28</v>
       </c>
@@ -1527,7 +1654,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
       <c r="B4" s="8"/>
       <c r="C4" s="19"/>
@@ -1568,14 +1695,14 @@
       <c r="AL4" s="20"/>
       <c r="AM4" s="22"/>
     </row>
-    <row r="5" spans="1:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="54" t="s">
+    <row r="5" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="57" t="s">
+      <c r="C5" s="61" t="s">
         <v>33</v>
       </c>
       <c r="D5" s="11" t="s">
@@ -1617,10 +1744,10 @@
       <c r="AL5" s="17"/>
       <c r="AM5" s="18"/>
     </row>
-    <row r="6" spans="1:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="55"/>
-      <c r="B6" s="56"/>
-      <c r="C6" s="57"/>
+    <row r="6" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="64"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="61"/>
       <c r="D6" s="11" t="s">
         <v>26</v>
       </c>
@@ -1660,10 +1787,10 @@
       <c r="AL6" s="17"/>
       <c r="AM6" s="18"/>
     </row>
-    <row r="7" spans="1:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="55"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="57"/>
+    <row r="7" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="64"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="61"/>
       <c r="D7" s="11" t="s">
         <v>32</v>
       </c>
@@ -1703,10 +1830,10 @@
       <c r="AL7" s="17"/>
       <c r="AM7" s="18"/>
     </row>
-    <row r="8" spans="1:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="55"/>
-      <c r="B8" s="56"/>
-      <c r="C8" s="57"/>
+    <row r="8" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="64"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="61"/>
       <c r="D8" s="11" t="s">
         <v>29</v>
       </c>
@@ -1746,10 +1873,10 @@
       <c r="AL8" s="17"/>
       <c r="AM8" s="18"/>
     </row>
-    <row r="9" spans="1:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="55"/>
-      <c r="B9" s="56"/>
-      <c r="C9" s="57"/>
+    <row r="9" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="64"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="61"/>
       <c r="D9" s="11" t="s">
         <v>31</v>
       </c>
@@ -1789,10 +1916,10 @@
       <c r="AL9" s="17"/>
       <c r="AM9" s="18"/>
     </row>
-    <row r="10" spans="1:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="55"/>
-      <c r="B10" s="56"/>
-      <c r="C10" s="57"/>
+    <row r="10" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="64"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="61"/>
       <c r="D10" s="11" t="s">
         <v>30</v>
       </c>
@@ -1832,10 +1959,10 @@
       <c r="AL10" s="17"/>
       <c r="AM10" s="18"/>
     </row>
-    <row r="11" spans="1:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="55"/>
-      <c r="B11" s="56"/>
-      <c r="C11" s="57"/>
+    <row r="11" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="64"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="61"/>
       <c r="D11" s="11" t="s">
         <v>28</v>
       </c>
@@ -1875,10 +2002,10 @@
       <c r="AL11" s="17"/>
       <c r="AM11" s="18"/>
     </row>
-    <row r="12" spans="1:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="55"/>
-      <c r="B12" s="56"/>
-      <c r="C12" s="57"/>
+    <row r="12" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="64"/>
+      <c r="B12" s="62"/>
+      <c r="C12" s="61"/>
       <c r="D12" s="11" t="s">
         <v>27</v>
       </c>
@@ -1917,11 +2044,14 @@
       <c r="AK12" s="17"/>
       <c r="AL12" s="17"/>
       <c r="AM12" s="18"/>
-    </row>
-    <row r="13" spans="1:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="55"/>
-      <c r="B13" s="56"/>
-      <c r="C13" s="57"/>
+      <c r="AO12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="64"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="61"/>
       <c r="D13" s="29" t="s">
         <v>38</v>
       </c>
@@ -1961,9 +2091,9 @@
       <c r="AL13" s="31"/>
       <c r="AM13" s="32"/>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A14" s="55"/>
-      <c r="B14" s="56"/>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A14" s="64"/>
+      <c r="B14" s="62"/>
       <c r="C14" s="23"/>
       <c r="D14" s="24"/>
       <c r="E14" s="25"/>
@@ -2002,10 +2132,10 @@
       <c r="AL14" s="25"/>
       <c r="AM14" s="26"/>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A15" s="55"/>
-      <c r="B15" s="56"/>
-      <c r="C15" s="57" t="s">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A15" s="64"/>
+      <c r="B15" s="62"/>
+      <c r="C15" s="61" t="s">
         <v>34</v>
       </c>
       <c r="D15" s="11" t="s">
@@ -2047,10 +2177,10 @@
       <c r="AL15" s="17"/>
       <c r="AM15" s="18"/>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A16" s="55"/>
-      <c r="B16" s="56"/>
-      <c r="C16" s="57"/>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A16" s="64"/>
+      <c r="B16" s="62"/>
+      <c r="C16" s="61"/>
       <c r="D16" s="11" t="s">
         <v>36</v>
       </c>
@@ -2095,15 +2225,15 @@
       <c r="AM17" s="10"/>
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A18" s="54" t="s">
+      <c r="A18" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="56" t="s">
+      <c r="B18" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="57"/>
+      <c r="C18" s="61"/>
       <c r="D18" s="11" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E18" s="27"/>
       <c r="F18" s="28"/>
@@ -2142,11 +2272,11 @@
       <c r="AM18" s="18"/>
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A19" s="55"/>
-      <c r="B19" s="56"/>
-      <c r="C19" s="57"/>
+      <c r="A19" s="64"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="61"/>
       <c r="D19" s="11" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="E19" s="27"/>
       <c r="F19" s="28"/>
@@ -2185,9 +2315,9 @@
       <c r="AM19" s="18"/>
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A20" s="55"/>
-      <c r="B20" s="56"/>
-      <c r="C20" s="57"/>
+      <c r="A20" s="64"/>
+      <c r="B20" s="62"/>
+      <c r="C20" s="61"/>
       <c r="D20" s="11" t="s">
         <v>32</v>
       </c>
@@ -2228,24 +2358,24 @@
       <c r="AM20" s="18"/>
     </row>
     <row r="21" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A21" s="55"/>
-      <c r="B21" s="56"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="64" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="65"/>
-      <c r="F21" s="65"/>
-      <c r="G21" s="65"/>
-      <c r="H21" s="65"/>
-      <c r="I21" s="65"/>
-      <c r="J21" s="65"/>
-      <c r="K21" s="65"/>
-      <c r="L21" s="65"/>
-      <c r="M21" s="65"/>
-      <c r="N21" s="65"/>
-      <c r="O21" s="65"/>
-      <c r="P21" s="65"/>
+      <c r="A21" s="64"/>
+      <c r="B21" s="62"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="50"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="50"/>
+      <c r="H21" s="50"/>
+      <c r="I21" s="50"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="50"/>
+      <c r="L21" s="50"/>
+      <c r="M21" s="50"/>
+      <c r="N21" s="50"/>
+      <c r="O21" s="50"/>
+      <c r="P21" s="50"/>
       <c r="Q21" s="43"/>
       <c r="R21" s="43"/>
       <c r="S21" s="43"/>
@@ -2271,11 +2401,11 @@
       <c r="AM21" s="44"/>
     </row>
     <row r="22" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A22" s="55"/>
-      <c r="B22" s="56"/>
-      <c r="C22" s="57"/>
-      <c r="D22" s="66" t="s">
-        <v>44</v>
+      <c r="A22" s="64"/>
+      <c r="B22" s="62"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="51" t="s">
+        <v>43</v>
       </c>
       <c r="E22" s="27"/>
       <c r="F22" s="28"/>
@@ -2314,11 +2444,11 @@
       <c r="AM22" s="44"/>
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A23" s="55"/>
-      <c r="B23" s="56"/>
-      <c r="C23" s="57"/>
+      <c r="A23" s="64"/>
+      <c r="B23" s="62"/>
+      <c r="C23" s="61"/>
       <c r="D23" s="42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E23" s="45"/>
       <c r="F23" s="46"/>
@@ -2357,9 +2487,9 @@
       <c r="AM23" s="44"/>
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A24" s="55"/>
-      <c r="B24" s="56"/>
-      <c r="C24" s="57"/>
+      <c r="A24" s="64"/>
+      <c r="B24" s="62"/>
+      <c r="C24" s="61"/>
       <c r="D24" s="11" t="s">
         <v>28</v>
       </c>
@@ -2400,18 +2530,18 @@
       <c r="AM24" s="44"/>
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A25" s="55"/>
-      <c r="B25" s="56"/>
-      <c r="C25" s="57"/>
+      <c r="A25" s="64"/>
+      <c r="B25" s="62"/>
+      <c r="C25" s="61"/>
     </row>
     <row r="26" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A26" s="55"/>
-      <c r="B26" s="56"/>
-      <c r="C26" s="57"/>
+      <c r="A26" s="64"/>
+      <c r="B26" s="62"/>
+      <c r="C26" s="61"/>
     </row>
     <row r="27" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A27" s="55"/>
-      <c r="B27" s="56"/>
+      <c r="A27" s="64"/>
+      <c r="B27" s="62"/>
       <c r="C27" s="23"/>
       <c r="D27" s="24"/>
       <c r="E27" s="25"/>
@@ -2451,11 +2581,11 @@
       <c r="AM27" s="26"/>
     </row>
     <row r="28" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A28" s="55"/>
-      <c r="B28" s="56"/>
-      <c r="C28" s="57"/>
+      <c r="A28" s="64"/>
+      <c r="B28" s="62"/>
+      <c r="C28" s="61"/>
       <c r="D28" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E28" s="30"/>
       <c r="F28" s="31"/>
@@ -2494,11 +2624,11 @@
       <c r="AM28" s="32"/>
     </row>
     <row r="29" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A29" s="55"/>
-      <c r="B29" s="56"/>
-      <c r="C29" s="57"/>
+      <c r="A29" s="64"/>
+      <c r="B29" s="62"/>
+      <c r="C29" s="61"/>
       <c r="D29" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E29" s="30"/>
       <c r="F29" s="31"/>
@@ -2538,12 +2668,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="I2:AM2"/>
-    <mergeCell ref="C2:D3"/>
-    <mergeCell ref="C5:C13"/>
-    <mergeCell ref="B5:B16"/>
-    <mergeCell ref="C15:C16"/>
     <mergeCell ref="A18:A29"/>
     <mergeCell ref="B18:B29"/>
     <mergeCell ref="C18:C26"/>
@@ -2551,10 +2675,17 @@
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A5:A16"/>
     <mergeCell ref="B2:B3"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="I2:AM2"/>
+    <mergeCell ref="C2:D3"/>
+    <mergeCell ref="C5:C13"/>
+    <mergeCell ref="B5:B16"/>
+    <mergeCell ref="C15:C16"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>